<commit_message>
These are changes (apparently) made on the 10 & 11th May 2020 - and it looks like they weren't committed nor pushed through then. Since, the computer died and been rebuilt. These are from the E drive backup on rainbow drive.
</commit_message>
<xml_diff>
--- a/data/methods.summary.xlsx
+++ b/data/methods.summary.xlsx
@@ -71,13 +71,13 @@
     <t>cart</t>
   </si>
   <si>
+    <t>rpart</t>
+  </si>
+  <si>
+    <t>glm</t>
+  </si>
+  <si>
     <t>mda</t>
-  </si>
-  <si>
-    <t>rpart</t>
-  </si>
-  <si>
-    <t>glm</t>
   </si>
   <si>
     <t>fda</t>
@@ -157,16 +157,16 @@
         <v>14</v>
       </c>
       <c r="C2" t="n">
-        <v>0.642462</v>
+        <v>0.76366</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0947172596444233</v>
+        <v>0.09844368297374326</v>
       </c>
       <c r="E2" t="n">
-        <v>0.87199</v>
+        <v>0.91752</v>
       </c>
       <c r="F2" t="n">
-        <v>0.04797061872147411</v>
+        <v>0.04317273874497056</v>
       </c>
     </row>
     <row r="3">
@@ -177,16 +177,16 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>0.636514</v>
+        <v>0.702136</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1006411002827983</v>
+        <v>0.1024775722273866</v>
       </c>
       <c r="E3" t="n">
-        <v>0.858372</v>
+        <v>0.884432</v>
       </c>
       <c r="F3" t="n">
-        <v>0.054062511283258986</v>
+        <v>0.052885755949638555</v>
       </c>
     </row>
     <row r="4">
@@ -197,16 +197,16 @@
         <v>16</v>
       </c>
       <c r="C4" t="n">
-        <v>0.624076</v>
+        <v>0.659018</v>
       </c>
       <c r="D4" t="n">
-        <v>0.10648837387970146</v>
+        <v>0.09889014205871476</v>
       </c>
       <c r="E4" t="n">
-        <v>0.83076</v>
+        <v>0.8604</v>
       </c>
       <c r="F4" t="n">
-        <v>0.06245670564607391</v>
+        <v>0.05721215308762505</v>
       </c>
     </row>
     <row r="5">
@@ -217,16 +217,16 @@
         <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6035791583166332</v>
+        <v>0.64745</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1140063552731322</v>
+        <v>0.13654052192758204</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8259939879759519</v>
+        <v>0.82966</v>
       </c>
       <c r="F5" t="n">
-        <v>0.06956336832542664</v>
+        <v>0.08167161628014731</v>
       </c>
     </row>
     <row r="6">
@@ -237,16 +237,16 @@
         <v>18</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5634854368932039</v>
+        <v>0.6448989898989899</v>
       </c>
       <c r="D6" t="n">
-        <v>0.11751911518087382</v>
+        <v>0.1313711438937367</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8040873786407767</v>
+        <v>0.833939393939394</v>
       </c>
       <c r="F6" t="n">
-        <v>0.06860859529930241</v>
+        <v>0.0785287959899357</v>
       </c>
     </row>
     <row r="7">
@@ -257,16 +257,16 @@
         <v>19</v>
       </c>
       <c r="C7" t="n">
-        <v>0.54181</v>
+        <v>0.603202</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1157853808078448</v>
+        <v>0.11489342101436778</v>
       </c>
       <c r="E7" t="n">
-        <v>0.781412</v>
+        <v>0.830688</v>
       </c>
       <c r="F7" t="n">
-        <v>0.07176119839572344</v>
+        <v>0.06932594629472662</v>
       </c>
     </row>
     <row r="8">
@@ -277,16 +277,16 @@
         <v>20</v>
       </c>
       <c r="C8" t="n">
-        <v>0.538038</v>
+        <v>0.55956</v>
       </c>
       <c r="D8" t="n">
-        <v>0.10941125262239164</v>
+        <v>0.10843905411296166</v>
       </c>
       <c r="E8" t="n">
-        <v>0.79839</v>
+        <v>0.794496</v>
       </c>
       <c r="F8" t="n">
-        <v>0.06742918723061374</v>
+        <v>0.06514674343634316</v>
       </c>
     </row>
     <row r="9">
@@ -297,16 +297,16 @@
         <v>21</v>
       </c>
       <c r="C9" t="n">
-        <v>0.506162</v>
+        <v>0.557744</v>
       </c>
       <c r="D9" t="n">
-        <v>0.11110487091339138</v>
+        <v>0.11386531114507319</v>
       </c>
       <c r="E9" t="n">
-        <v>0.75649</v>
+        <v>0.792884</v>
       </c>
       <c r="F9" t="n">
-        <v>0.07220130162200557</v>
+        <v>0.07078737351037255</v>
       </c>
     </row>
     <row r="10">
@@ -317,16 +317,16 @@
         <v>22</v>
       </c>
       <c r="C10" t="n">
-        <v>0.458348</v>
+        <v>0.502652</v>
       </c>
       <c r="D10" t="n">
-        <v>0.11708730832820048</v>
+        <v>0.11640818109244085</v>
       </c>
       <c r="E10" t="n">
-        <v>0.72647</v>
+        <v>0.762462</v>
       </c>
       <c r="F10" t="n">
-        <v>0.07915959564807246</v>
+        <v>0.07569885858043543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>